<commit_message>
team member report and sprint backlog pushed
</commit_message>
<xml_diff>
--- a/docs/deliverable3/Getana_Deliverable_3_SprintBacklog_4.xlsx
+++ b/docs/deliverable3/Getana_Deliverable_3_SprintBacklog_4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Desktop\software\RaiderNAV\docs\deliverable3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC3B56-D795-4C20-9E8A-F111599E90CB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B07126F-C947-4C21-8B77-CCFF5C055AE2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="121">
   <si>
     <t>SPRINT BACKLOG — Deliverable 1</t>
   </si>
@@ -356,6 +356,42 @@
   </si>
   <si>
     <t>118, Create Sprint 5 review document</t>
+  </si>
+  <si>
+    <t>144, Update SRS and UC document document for User story 30</t>
+  </si>
+  <si>
+    <t>148, Update SRS and UC document document for User story 24</t>
+  </si>
+  <si>
+    <t>162, Restructure URN document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164,Create use case maps for schedule actions </t>
+  </si>
+  <si>
+    <t>119, Update Configuration management plan document</t>
+  </si>
+  <si>
+    <t>114, Update Platform Document</t>
+  </si>
+  <si>
+    <t>140, update grl and ucm model document for user story #24</t>
+  </si>
+  <si>
+    <t>137, update grl and ucm model document for user story #21</t>
+  </si>
+  <si>
+    <t>138, update grl and ucm model document for user story #30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T </t>
+  </si>
+  <si>
+    <t>160, Add unscheduled navigation scenario to URN document</t>
+  </si>
+  <si>
+    <t>161, Add edit course scenario to URN document</t>
   </si>
 </sst>
 </file>
@@ -2130,10 +2166,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2396,6 +2432,9 @@
       <c r="E19" s="6">
         <v>2</v>
       </c>
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
@@ -2413,6 +2452,9 @@
       <c r="E20" s="6">
         <v>2</v>
       </c>
+      <c r="G20" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
@@ -2435,6 +2477,259 @@
       </c>
       <c r="G21" s="6" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="6">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="6">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="6">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="6">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3</v>
+      </c>
+      <c r="F24" s="6">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="6">
+        <v>5</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="6">
+        <v>24</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>2</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="6">
+        <v>21</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="6">
+        <v>2</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="6">
+        <v>30</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="6">
+        <v>2</v>
+      </c>
+      <c r="F30" s="6">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6">
+        <v>2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="6">
+        <v>2</v>
+      </c>
+      <c r="F32" s="6">
+        <v>2</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>